<commit_message>
sales report pdf  format bug fix
</commit_message>
<xml_diff>
--- a/public/salesreport.xlsx
+++ b/public/salesreport.xlsx
@@ -365,25 +365,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D2" t="str">
-        <v>2023-11-08</v>
+        <v>2023-11-24</v>
       </c>
       <c r="E2" t="str">
         <v>COD</v>
       </c>
       <c r="F2">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="G2">
-        <v>2599</v>
+        <v>1389</v>
       </c>
       <c r="H2" t="str">
         <v>delivered</v>
@@ -391,25 +391,25 @@
     </row>
     <row r="3">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
       <c r="C3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="str">
-        <v>2023-11-07</v>
+        <v>2023-11-08</v>
       </c>
       <c r="E3" t="str">
-        <v>RAZOR PAY</v>
+        <v>COD</v>
       </c>
       <c r="F3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3">
-        <v>4488</v>
+        <v>2599</v>
       </c>
       <c r="H3" t="str">
         <v>delivered</v>
@@ -423,19 +423,19 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" t="str">
-        <v>2023-11-01</v>
+        <v>2023-11-07</v>
       </c>
       <c r="E4" t="str">
         <v>RAZOR PAY</v>
       </c>
       <c r="F4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4">
-        <v>999</v>
+        <v>4488</v>
       </c>
       <c r="H4" t="str">
         <v>delivered</v>
@@ -443,25 +443,25 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" t="str">
-        <v>2023-11-08</v>
+        <v>2023-11-01</v>
       </c>
       <c r="E5" t="str">
-        <v>COD</v>
+        <v>RAZOR PAY</v>
       </c>
       <c r="F5">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G5">
-        <v>2188</v>
+        <v>999</v>
       </c>
       <c r="H5" t="str">
         <v>delivered</v>
@@ -469,25 +469,25 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D6" t="str">
-        <v>2023-10-29</v>
+        <v>2023-11-08</v>
       </c>
       <c r="E6" t="str">
         <v>COD</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="G6">
-        <v>2496</v>
+        <v>2188</v>
       </c>
       <c r="H6" t="str">
         <v>delivered</v>
@@ -501,19 +501,19 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="str">
         <v>2023-10-29</v>
       </c>
       <c r="E7" t="str">
-        <v>RAZOR PAY</v>
+        <v>COD</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>999</v>
+        <v>2496</v>
       </c>
       <c r="H7" t="str">
         <v>delivered</v>
@@ -527,7 +527,7 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D8" t="str">
         <v>2023-10-29</v>
@@ -536,10 +536,10 @@
         <v>RAZOR PAY</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G8">
-        <v>698</v>
+        <v>999</v>
       </c>
       <c r="H8" t="str">
         <v>delivered</v>
@@ -553,7 +553,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D9" t="str">
         <v>2023-10-29</v>
@@ -562,12 +562,38 @@
         <v>RAZOR PAY</v>
       </c>
       <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>698</v>
+      </c>
+      <c r="H9" t="str">
+        <v>delivered</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
         <v>8</v>
       </c>
-      <c r="G9">
+      <c r="D10" t="str">
+        <v>2023-10-29</v>
+      </c>
+      <c r="E10" t="str">
+        <v>RAZOR PAY</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
         <v>999</v>
       </c>
-      <c r="H9" t="str">
+      <c r="H10" t="str">
         <v>delivered</v>
       </c>
     </row>

</xml_diff>